<commit_message>
Update client and import
</commit_message>
<xml_diff>
--- a/Akrapovic/akrapovik_code/akrapovic_catalogue.xlsx
+++ b/Akrapovic/akrapovik_code/akrapovic_catalogue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edmilbe\Documents\catalogos\AKRAPOVIC\akrapovik_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{498C26D4-8045-4B39-A798-C7363053DC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8B8E89-CB77-4F9D-A344-D3EF6600E8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prices - 31 August 2023" sheetId="1" r:id="rId1"/>
@@ -4511,21 +4511,20 @@
   <dimension ref="A1:S816"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A816" sqref="A1:A816"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="56.28515625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.85546875" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="12" width="11" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="56.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="13" width="11" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="14" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="108.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.28515625" style="4" bestFit="1" customWidth="1"/>

</xml_diff>